<commit_message>
'Wind Gap Simulado': V_sur - V_norte
</commit_message>
<xml_diff>
--- a/simulacion_viento.xlsx
+++ b/simulacion_viento.xlsx
@@ -491,7 +491,7 @@
         <v>7.121387474164425</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.2118984687569423</v>
+        <v>0.2118984687569423</v>
       </c>
     </row>
     <row r="4">
@@ -508,7 +508,7 @@
         <v>7.226583389284458</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.06546073798616803</v>
+        <v>0.06546073798616803</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,7 @@
         <v>8.003549922734317</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.05013356738812469</v>
+        <v>0.05013356738812469</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>9.25876765237415</v>
       </c>
       <c r="E6" t="n">
-        <v>0.008097674660540122</v>
+        <v>-0.008097674660540122</v>
       </c>
     </row>
     <row r="7">
@@ -559,7 +559,7 @@
         <v>8.887582702171576</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.4012289750622919</v>
+        <v>0.4012289750622919</v>
       </c>
     </row>
     <row r="8">
@@ -576,7 +576,7 @@
         <v>8.450184633499799</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.3351022244029132</v>
+        <v>0.3351022244029132</v>
       </c>
     </row>
     <row r="9">
@@ -593,7 +593,7 @@
         <v>9.534579258797395</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.02767491610618222</v>
+        <v>0.02767491610618222</v>
       </c>
     </row>
     <row r="10">
@@ -610,7 +610,7 @@
         <v>9.334508622938756</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7423926861061254</v>
+        <v>-0.7423926861061254</v>
       </c>
     </row>
     <row r="11">
@@ -627,7 +627,7 @@
         <v>8.220218519849865</v>
       </c>
       <c r="E11" t="n">
-        <v>1.150614307330599</v>
+        <v>-1.150614307330599</v>
       </c>
     </row>
     <row r="12">
@@ -644,7 +644,7 @@
         <v>7.938214271459177</v>
       </c>
       <c r="E12" t="n">
-        <v>2.135273198004704</v>
+        <v>-2.135273198004704</v>
       </c>
     </row>
     <row r="13">
@@ -661,7 +661,7 @@
         <v>7.583485712702701</v>
       </c>
       <c r="E13" t="n">
-        <v>1.446984219157733</v>
+        <v>-1.446984219157733</v>
       </c>
     </row>
     <row r="14">
@@ -678,7 +678,7 @@
         <v>6.955472362406628</v>
       </c>
       <c r="E14" t="n">
-        <v>1.715892264997208</v>
+        <v>-1.715892264997208</v>
       </c>
     </row>
     <row r="15">
@@ -695,7 +695,7 @@
         <v>7.267025499297399</v>
       </c>
       <c r="E15" t="n">
-        <v>1.585283553223349</v>
+        <v>-1.585283553223349</v>
       </c>
     </row>
     <row r="16">
@@ -712,7 +712,7 @@
         <v>5.154722138246205</v>
       </c>
       <c r="E16" t="n">
-        <v>2.531668473848942</v>
+        <v>-2.531668473848942</v>
       </c>
     </row>
     <row r="17">
@@ -729,7 +729,7 @@
         <v>4.543042542332942</v>
       </c>
       <c r="E17" t="n">
-        <v>1.769210616622944</v>
+        <v>-1.769210616622944</v>
       </c>
     </row>
     <row r="18">
@@ -746,7 +746,7 @@
         <v>5.159780672633615</v>
       </c>
       <c r="E18" t="n">
-        <v>1.091219109730241</v>
+        <v>-1.091219109730241</v>
       </c>
     </row>
     <row r="19">
@@ -763,7 +763,7 @@
         <v>5.204040672063151</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6300201812696589</v>
+        <v>-0.6300201812696589</v>
       </c>
     </row>
     <row r="20">
@@ -780,7 +780,7 @@
         <v>6.787351697641441</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.5751908108671575</v>
+        <v>0.5751908108671575</v>
       </c>
     </row>
     <row r="21">
@@ -797,7 +797,7 @@
         <v>6.546098056640108</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.7766199413572163</v>
+        <v>0.7766199413572163</v>
       </c>
     </row>
     <row r="22">
@@ -814,7 +814,7 @@
         <v>6.028836718659147</v>
       </c>
       <c r="E22" t="n">
-        <v>-1.074604893160794</v>
+        <v>1.074604893160794</v>
       </c>
     </row>
     <row r="23">
@@ -831,7 +831,7 @@
         <v>7.863852249364422</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.8527400396631499</v>
+        <v>0.8527400396631499</v>
       </c>
     </row>
     <row r="24">
@@ -848,7 +848,7 @@
         <v>7.657167595985662</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.5592178969207442</v>
+        <v>0.5592178969207442</v>
       </c>
     </row>
     <row r="25">
@@ -865,7 +865,7 @@
         <v>7.325200602513257</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5057762806509878</v>
+        <v>-0.5057762806509878</v>
       </c>
     </row>
     <row r="26">
@@ -882,7 +882,7 @@
         <v>5.991510657704546</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9406885185851781</v>
+        <v>-0.9406885185851781</v>
       </c>
     </row>
     <row r="27">
@@ -899,7 +899,7 @@
         <v>6.159020480927797</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5113193273952454</v>
+        <v>-0.5113193273952454</v>
       </c>
     </row>
     <row r="28">
@@ -916,7 +916,7 @@
         <v>6.9430490022101</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.03093899576710513</v>
+        <v>0.03093899576710513</v>
       </c>
     </row>
     <row r="29">
@@ -933,7 +933,7 @@
         <v>6.106688420265666</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2329615072569347</v>
+        <v>-0.2329615072569347</v>
       </c>
     </row>
     <row r="30">
@@ -950,7 +950,7 @@
         <v>7.25434098511745</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.4951780805901187</v>
+        <v>0.4951780805901187</v>
       </c>
     </row>
     <row r="31">
@@ -967,7 +967,7 @@
         <v>6.462624331631087</v>
       </c>
       <c r="E31" t="n">
-        <v>0.537713751770184</v>
+        <v>-0.537713751770184</v>
       </c>
     </row>
     <row r="32">
@@ -984,7 +984,7 @@
         <v>6.248428962649442</v>
       </c>
       <c r="E32" t="n">
-        <v>1.089344197882562</v>
+        <v>-1.089344197882562</v>
       </c>
     </row>
     <row r="33">
@@ -1001,7 +1001,7 @@
         <v>6.222413740249181</v>
       </c>
       <c r="E33" t="n">
-        <v>0.697165902781375</v>
+        <v>-0.697165902781375</v>
       </c>
     </row>
     <row r="34">
@@ -1018,7 +1018,7 @@
         <v>8.620484637902676</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.3000078605973791</v>
+        <v>0.3000078605973791</v>
       </c>
     </row>
     <row r="35">
@@ -1035,7 +1035,7 @@
         <v>8.002467679712915</v>
       </c>
       <c r="E35" t="n">
-        <v>0.4547845963414332</v>
+        <v>-0.4547845963414332</v>
       </c>
     </row>
     <row r="36">
@@ -1052,7 +1052,7 @@
         <v>7.012068976786762</v>
       </c>
       <c r="E36" t="n">
-        <v>0.3340113614344151</v>
+        <v>-0.3340113614344151</v>
       </c>
     </row>
     <row r="37">
@@ -1069,7 +1069,7 @@
         <v>7.543947304156061</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9434726352854339</v>
+        <v>-0.9434726352854339</v>
       </c>
     </row>
     <row r="38">
@@ -1086,7 +1086,7 @@
         <v>6.892466161518708</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.02365535754680081</v>
+        <v>0.02365535754680081</v>
       </c>
     </row>
     <row r="39">
@@ -1103,7 +1103,7 @@
         <v>7.448172076581836</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.3370706591584884</v>
+        <v>0.3370706591584884</v>
       </c>
     </row>
     <row r="40">
@@ -1120,7 +1120,7 @@
         <v>5.877369241030978</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.2896232559217182</v>
+        <v>0.2896232559217182</v>
       </c>
     </row>
     <row r="41">
@@ -1137,7 +1137,7 @@
         <v>5.285563110558184</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.2264222048915503</v>
+        <v>0.2264222048915503</v>
       </c>
     </row>
     <row r="42">
@@ -1154,7 +1154,7 @@
         <v>6.270864681312801</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.434105616698897</v>
+        <v>0.434105616698897</v>
       </c>
     </row>
     <row r="43">
@@ -1171,7 +1171,7 @@
         <v>7.14358243228616</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.0476171234359537</v>
+        <v>0.0476171234359537</v>
       </c>
     </row>
     <row r="44">
@@ -1188,7 +1188,7 @@
         <v>7.686637031351566</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.6051530072096725</v>
+        <v>0.6051530072096725</v>
       </c>
     </row>
     <row r="45">
@@ -1205,7 +1205,7 @@
         <v>7.621619699010183</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.6001367715722505</v>
+        <v>0.6001367715722505</v>
       </c>
     </row>
     <row r="46">
@@ -1222,7 +1222,7 @@
         <v>7.34368906384802</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.4570575737341986</v>
+        <v>0.4570575737341986</v>
       </c>
     </row>
     <row r="47">
@@ -1239,7 +1239,7 @@
         <v>6.037373750784536</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.1247825127072595</v>
+        <v>0.1247825127072595</v>
       </c>
     </row>
     <row r="48">
@@ -1256,7 +1256,7 @@
         <v>5.671982388933744</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2675856900702733</v>
+        <v>-0.2675856900702733</v>
       </c>
     </row>
     <row r="49">
@@ -1273,7 +1273,7 @@
         <v>6.078471486302385</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.3618447997117507</v>
+        <v>0.3618447997117507</v>
       </c>
     </row>
     <row r="50">
@@ -1290,7 +1290,7 @@
         <v>7.790791472405498</v>
       </c>
       <c r="E50" t="n">
-        <v>-1.124102000486872</v>
+        <v>1.124102000486872</v>
       </c>
     </row>
     <row r="51">
@@ -1307,7 +1307,7 @@
         <v>7.705238529016647</v>
       </c>
       <c r="E51" t="n">
-        <v>-0.300319076674965</v>
+        <v>0.300319076674965</v>
       </c>
     </row>
     <row r="52">
@@ -1324,7 +1324,7 @@
         <v>6.049951405524171</v>
       </c>
       <c r="E52" t="n">
-        <v>-0.08500582654050426</v>
+        <v>0.08500582654050426</v>
       </c>
     </row>
     <row r="53">
@@ -1341,7 +1341,7 @@
         <v>6.9019352928667</v>
       </c>
       <c r="E53" t="n">
-        <v>-0.4690402197031958</v>
+        <v>0.4690402197031958</v>
       </c>
     </row>
     <row r="54">
@@ -1358,7 +1358,7 @@
         <v>6.320477598017656</v>
       </c>
       <c r="E54" t="n">
-        <v>0.4123473396628015</v>
+        <v>-0.4123473396628015</v>
       </c>
     </row>
     <row r="55">
@@ -1375,7 +1375,7 @@
         <v>5.965610454990582</v>
       </c>
       <c r="E55" t="n">
-        <v>0.4187833397427401</v>
+        <v>-0.4187833397427401</v>
       </c>
     </row>
     <row r="56">
@@ -1392,7 +1392,7 @@
         <v>6.509295187368929</v>
       </c>
       <c r="E56" t="n">
-        <v>0.9861022777776736</v>
+        <v>-0.9861022777776736</v>
       </c>
     </row>
     <row r="57">
@@ -1409,7 +1409,7 @@
         <v>7.480467478494002</v>
       </c>
       <c r="E57" t="n">
-        <v>0.8910553025782972</v>
+        <v>-0.8910553025782972</v>
       </c>
     </row>
     <row r="58">
@@ -1426,7 +1426,7 @@
         <v>7.550603790693139</v>
       </c>
       <c r="E58" t="n">
-        <v>1.861300318329271</v>
+        <v>-1.861300318329271</v>
       </c>
     </row>
     <row r="59">
@@ -1443,7 +1443,7 @@
         <v>6.104682267824397</v>
       </c>
       <c r="E59" t="n">
-        <v>2.541645261461963</v>
+        <v>-2.541645261461963</v>
       </c>
     </row>
     <row r="60">
@@ -1460,7 +1460,7 @@
         <v>6.000432784566688</v>
       </c>
       <c r="E60" t="n">
-        <v>2.073268789312057</v>
+        <v>-2.073268789312057</v>
       </c>
     </row>
     <row r="61">
@@ -1477,7 +1477,7 @@
         <v>6.173215691988836</v>
       </c>
       <c r="E61" t="n">
-        <v>2.311581640957333</v>
+        <v>-2.311581640957333</v>
       </c>
     </row>
     <row r="62">
@@ -1494,7 +1494,7 @@
         <v>6.892794053621945</v>
       </c>
       <c r="E62" t="n">
-        <v>2.346031702250666</v>
+        <v>-2.346031702250666</v>
       </c>
     </row>
     <row r="63">
@@ -1511,7 +1511,7 @@
         <v>5.973069725246937</v>
       </c>
       <c r="E63" t="n">
-        <v>2.757891889640581</v>
+        <v>-2.757891889640581</v>
       </c>
     </row>
     <row r="64">
@@ -1528,7 +1528,7 @@
         <v>6.147963810619562</v>
       </c>
       <c r="E64" t="n">
-        <v>1.882729387629078</v>
+        <v>-1.882729387629078</v>
       </c>
     </row>
     <row r="65">
@@ -1545,7 +1545,7 @@
         <v>5.125532989809848</v>
       </c>
       <c r="E65" t="n">
-        <v>1.995505083928618</v>
+        <v>-1.995505083928618</v>
       </c>
     </row>
     <row r="66">
@@ -1562,7 +1562,7 @@
         <v>4.216771286146627</v>
       </c>
       <c r="E66" t="n">
-        <v>2.28999572434919</v>
+        <v>-2.28999572434919</v>
       </c>
     </row>
     <row r="67">
@@ -1579,7 +1579,7 @@
         <v>5.976625144785846</v>
       </c>
       <c r="E67" t="n">
-        <v>1.057610078872306</v>
+        <v>-1.057610078872306</v>
       </c>
     </row>
     <row r="68">
@@ -1596,7 +1596,7 @@
         <v>7.607907645291086</v>
       </c>
       <c r="E68" t="n">
-        <v>0.2925061116421546</v>
+        <v>-0.2925061116421546</v>
       </c>
     </row>
     <row r="69">
@@ -1613,7 +1613,7 @@
         <v>7.832467065681849</v>
       </c>
       <c r="E69" t="n">
-        <v>-0.8232543241214323</v>
+        <v>0.8232543241214323</v>
       </c>
     </row>
     <row r="70">
@@ -1630,7 +1630,7 @@
         <v>8.50907449327692</v>
       </c>
       <c r="E70" t="n">
-        <v>-0.8564167629737121</v>
+        <v>0.8564167629737121</v>
       </c>
     </row>
     <row r="71">
@@ -1647,7 +1647,7 @@
         <v>8.177008915498892</v>
       </c>
       <c r="E71" t="n">
-        <v>-0.3639414896096875</v>
+        <v>0.3639414896096875</v>
       </c>
     </row>
     <row r="72">
@@ -1664,7 +1664,7 @@
         <v>6.841252749280015</v>
       </c>
       <c r="E72" t="n">
-        <v>0.4777451549443228</v>
+        <v>-0.4777451549443228</v>
       </c>
     </row>
     <row r="73">
@@ -1681,7 +1681,7 @@
         <v>7.047637555840093</v>
       </c>
       <c r="E73" t="n">
-        <v>0.4535530437608557</v>
+        <v>-0.4535530437608557</v>
       </c>
     </row>
     <row r="74">
@@ -1698,7 +1698,7 @@
         <v>7.762012504919626</v>
       </c>
       <c r="E74" t="n">
-        <v>1.253563964058279</v>
+        <v>-1.253563964058279</v>
       </c>
     </row>
     <row r="75">
@@ -1715,7 +1715,7 @@
         <v>7.659400260485661</v>
       </c>
       <c r="E75" t="n">
-        <v>0.3585271145379245</v>
+        <v>-0.3585271145379245</v>
       </c>
     </row>
     <row r="76">
@@ -1732,7 +1732,7 @@
         <v>9.081380821832104</v>
       </c>
       <c r="E76" t="n">
-        <v>-0.5886103559357956</v>
+        <v>0.5886103559357956</v>
       </c>
     </row>
     <row r="77">
@@ -1749,7 +1749,7 @@
         <v>6.198761990313351</v>
       </c>
       <c r="E77" t="n">
-        <v>-0.5399279321271937</v>
+        <v>0.5399279321271937</v>
       </c>
     </row>
     <row r="78">
@@ -1766,7 +1766,7 @@
         <v>6.938129450695591</v>
       </c>
       <c r="E78" t="n">
-        <v>-0.2655232889551709</v>
+        <v>0.2655232889551709</v>
       </c>
     </row>
     <row r="79">
@@ -1783,7 +1783,7 @@
         <v>6.916572305085482</v>
       </c>
       <c r="E79" t="n">
-        <v>-0.2475959548151305</v>
+        <v>0.2475959548151305</v>
       </c>
     </row>
     <row r="80">
@@ -1800,7 +1800,7 @@
         <v>7.10319045480199</v>
       </c>
       <c r="E80" t="n">
-        <v>-1.306665611377797</v>
+        <v>1.306665611377797</v>
       </c>
     </row>
     <row r="81">
@@ -1817,7 +1817,7 @@
         <v>7.117876234920383</v>
       </c>
       <c r="E81" t="n">
-        <v>-1.180537158228155</v>
+        <v>1.180537158228155</v>
       </c>
     </row>
     <row r="82">
@@ -1834,7 +1834,7 @@
         <v>5.682791100105559</v>
       </c>
       <c r="E82" t="n">
-        <v>-1.712995041405527</v>
+        <v>1.712995041405527</v>
       </c>
     </row>
     <row r="83">
@@ -1851,7 +1851,7 @@
         <v>5.674339613629527</v>
       </c>
       <c r="E83" t="n">
-        <v>-1.132263732469207</v>
+        <v>1.132263732469207</v>
       </c>
     </row>
     <row r="84">
@@ -1868,7 +1868,7 @@
         <v>6.174184165581857</v>
       </c>
       <c r="E84" t="n">
-        <v>-0.7885712326851415</v>
+        <v>0.7885712326851415</v>
       </c>
     </row>
     <row r="85">
@@ -1885,7 +1885,7 @@
         <v>7.771651650705448</v>
       </c>
       <c r="E85" t="n">
-        <v>-1.180430900747995</v>
+        <v>1.180430900747995</v>
       </c>
     </row>
     <row r="86">
@@ -1902,7 +1902,7 @@
         <v>7.12519722030274</v>
       </c>
       <c r="E86" t="n">
-        <v>-1.295358180096564</v>
+        <v>1.295358180096564</v>
       </c>
     </row>
     <row r="87">
@@ -1919,7 +1919,7 @@
         <v>6.571877561801896</v>
       </c>
       <c r="E87" t="n">
-        <v>-1.683068570775754</v>
+        <v>1.683068570775754</v>
       </c>
     </row>
     <row r="88">
@@ -1936,7 +1936,7 @@
         <v>6.200565219188166</v>
       </c>
       <c r="E88" t="n">
-        <v>-1.493084298689274</v>
+        <v>1.493084298689274</v>
       </c>
     </row>
     <row r="89">
@@ -1953,7 +1953,7 @@
         <v>6.835303474378121</v>
       </c>
       <c r="E89" t="n">
-        <v>-0.7907352037905113</v>
+        <v>0.7907352037905113</v>
       </c>
     </row>
     <row r="90">
@@ -1970,7 +1970,7 @@
         <v>7.231316315203173</v>
       </c>
       <c r="E90" t="n">
-        <v>-1.206521044442686</v>
+        <v>1.206521044442686</v>
       </c>
     </row>
     <row r="91">
@@ -1987,7 +1987,7 @@
         <v>6.419024921506686</v>
       </c>
       <c r="E91" t="n">
-        <v>-0.7803946847954784</v>
+        <v>0.7803946847954784</v>
       </c>
     </row>
     <row r="92">
@@ -2004,7 +2004,7 @@
         <v>6.952800218203236</v>
       </c>
       <c r="E92" t="n">
-        <v>-0.9570024411717331</v>
+        <v>0.9570024411717331</v>
       </c>
     </row>
     <row r="93">
@@ -2021,7 +2021,7 @@
         <v>7.051213906401116</v>
       </c>
       <c r="E93" t="n">
-        <v>-1.248897419487562</v>
+        <v>1.248897419487562</v>
       </c>
     </row>
     <row r="94">
@@ -2038,7 +2038,7 @@
         <v>7.684839722497722</v>
       </c>
       <c r="E94" t="n">
-        <v>-1.139885083863311</v>
+        <v>1.139885083863311</v>
       </c>
     </row>
     <row r="95">
@@ -2055,7 +2055,7 @@
         <v>6.951935617518856</v>
       </c>
       <c r="E95" t="n">
-        <v>-1.535543090834095</v>
+        <v>1.535543090834095</v>
       </c>
     </row>
     <row r="96">
@@ -2072,7 +2072,7 @@
         <v>6.648146617657157</v>
       </c>
       <c r="E96" t="n">
-        <v>-1.624411440134031</v>
+        <v>1.624411440134031</v>
       </c>
     </row>
     <row r="97">
@@ -2089,7 +2089,7 @@
         <v>6.548377611528253</v>
       </c>
       <c r="E97" t="n">
-        <v>-2.041739968406851</v>
+        <v>2.041739968406851</v>
       </c>
     </row>
     <row r="98">
@@ -2106,7 +2106,7 @@
         <v>4.768287209245814</v>
       </c>
       <c r="E98" t="n">
-        <v>-0.7334719378450032</v>
+        <v>0.7334719378450032</v>
       </c>
     </row>
     <row r="99">
@@ -2123,7 +2123,7 @@
         <v>5.388368019127745</v>
       </c>
       <c r="E99" t="n">
-        <v>-0.6176278328399842</v>
+        <v>0.6176278328399842</v>
       </c>
     </row>
     <row r="100">
@@ -2140,7 +2140,7 @@
         <v>5.967652134588701</v>
       </c>
       <c r="E100" t="n">
-        <v>-0.9053118804564093</v>
+        <v>0.9053118804564093</v>
       </c>
     </row>
     <row r="101">
@@ -2157,7 +2157,7 @@
         <v>5.931180783955883</v>
       </c>
       <c r="E101" t="n">
-        <v>-0.6723044268617056</v>
+        <v>0.6723044268617056</v>
       </c>
     </row>
     <row r="102">
@@ -2174,7 +2174,7 @@
         <v>5.760906101830271</v>
       </c>
       <c r="E102" t="n">
-        <v>-0.6425162016101957</v>
+        <v>0.6425162016101957</v>
       </c>
     </row>
     <row r="103">
@@ -2191,7 +2191,7 @@
         <v>4.666234850376505</v>
       </c>
       <c r="E103" t="n">
-        <v>-0.6740537208574509</v>
+        <v>0.6740537208574509</v>
       </c>
     </row>
     <row r="104">
@@ -2208,7 +2208,7 @@
         <v>4.506163825924406</v>
       </c>
       <c r="E104" t="n">
-        <v>-0.2603465160493208</v>
+        <v>0.2603465160493208</v>
       </c>
     </row>
     <row r="105">
@@ -2225,7 +2225,7 @@
         <v>4.376948948400668</v>
       </c>
       <c r="E105" t="n">
-        <v>0.1742280155925791</v>
+        <v>-0.1742280155925791</v>
       </c>
     </row>
     <row r="106">
@@ -2242,7 +2242,7 @@
         <v>4.194359934395633</v>
       </c>
       <c r="E106" t="n">
-        <v>-0.1290416344169447</v>
+        <v>0.1290416344169447</v>
       </c>
     </row>
     <row r="107">
@@ -2259,7 +2259,7 @@
         <v>4.631726093995276</v>
       </c>
       <c r="E107" t="n">
-        <v>-0.4160470465262112</v>
+        <v>0.4160470465262112</v>
       </c>
     </row>
     <row r="108">
@@ -2276,7 +2276,7 @@
         <v>5.347329566796343</v>
       </c>
       <c r="E108" t="n">
-        <v>-0.506165221382707</v>
+        <v>0.506165221382707</v>
       </c>
     </row>
     <row r="109">
@@ -2293,7 +2293,7 @@
         <v>7.625926455369965</v>
       </c>
       <c r="E109" t="n">
-        <v>-1.654798592343139</v>
+        <v>1.654798592343139</v>
       </c>
     </row>
     <row r="110">
@@ -2310,7 +2310,7 @@
         <v>7.663752817918425</v>
       </c>
       <c r="E110" t="n">
-        <v>-2.235683473691982</v>
+        <v>2.235683473691982</v>
       </c>
     </row>
     <row r="111">
@@ -2327,7 +2327,7 @@
         <v>7.037367149850878</v>
       </c>
       <c r="E111" t="n">
-        <v>-1.217454440154041</v>
+        <v>1.217454440154041</v>
       </c>
     </row>
     <row r="112">
@@ -2344,7 +2344,7 @@
         <v>6.151531321992636</v>
       </c>
       <c r="E112" t="n">
-        <v>-0.1873187635170233</v>
+        <v>0.1873187635170233</v>
       </c>
     </row>
     <row r="113">
@@ -2361,7 +2361,7 @@
         <v>4.386806377616411</v>
       </c>
       <c r="E113" t="n">
-        <v>-0.29401462979156</v>
+        <v>0.29401462979156</v>
       </c>
     </row>
     <row r="114">
@@ -2378,7 +2378,7 @@
         <v>4.519921066736465</v>
       </c>
       <c r="E114" t="n">
-        <v>0.04945616581180445</v>
+        <v>-0.04945616581180445</v>
       </c>
     </row>
     <row r="115">
@@ -2395,7 +2395,7 @@
         <v>4.717791390021076</v>
       </c>
       <c r="E115" t="n">
-        <v>0.2072828714448782</v>
+        <v>-0.2072828714448782</v>
       </c>
     </row>
     <row r="116">
@@ -2412,7 +2412,7 @@
         <v>6.120347322921358</v>
       </c>
       <c r="E116" t="n">
-        <v>1.805871861537481</v>
+        <v>-1.805871861537481</v>
       </c>
     </row>
     <row r="117">
@@ -2429,7 +2429,7 @@
         <v>5.248306580651567</v>
       </c>
       <c r="E117" t="n">
-        <v>2.157793659388961</v>
+        <v>-2.157793659388961</v>
       </c>
     </row>
     <row r="118">
@@ -2446,7 +2446,7 @@
         <v>5.342466667173955</v>
       </c>
       <c r="E118" t="n">
-        <v>1.804224820010877</v>
+        <v>-1.804224820010877</v>
       </c>
     </row>
     <row r="119">
@@ -2463,7 +2463,7 @@
         <v>5.364733986569496</v>
       </c>
       <c r="E119" t="n">
-        <v>1.06042442728654</v>
+        <v>-1.06042442728654</v>
       </c>
     </row>
     <row r="120">
@@ -2480,7 +2480,7 @@
         <v>4.652812291372393</v>
       </c>
       <c r="E120" t="n">
-        <v>0.07144724211475939</v>
+        <v>-0.07144724211475939</v>
       </c>
     </row>
     <row r="121">
@@ -2497,7 +2497,7 @@
         <v>5.689777750209067</v>
       </c>
       <c r="E121" t="n">
-        <v>0.1694332709814486</v>
+        <v>-0.1694332709814486</v>
       </c>
     </row>
     <row r="122">
@@ -2514,7 +2514,7 @@
         <v>6.324399622407393</v>
       </c>
       <c r="E122" t="n">
-        <v>-0.2524798635528835</v>
+        <v>0.2524798635528835</v>
       </c>
     </row>
     <row r="123">
@@ -2531,7 +2531,7 @@
         <v>7.003859433767468</v>
       </c>
       <c r="E123" t="n">
-        <v>-0.9701557665696505</v>
+        <v>0.9701557665696505</v>
       </c>
     </row>
     <row r="124">
@@ -2548,7 +2548,7 @@
         <v>5.898345132152569</v>
       </c>
       <c r="E124" t="n">
-        <v>-1.183041213930084</v>
+        <v>1.183041213930084</v>
       </c>
     </row>
     <row r="125">
@@ -2565,7 +2565,7 @@
         <v>7.188516283888392</v>
       </c>
       <c r="E125" t="n">
-        <v>-1.59743460333841</v>
+        <v>1.59743460333841</v>
       </c>
     </row>
     <row r="126">
@@ -2582,7 +2582,7 @@
         <v>5.032523648749558</v>
       </c>
       <c r="E126" t="n">
-        <v>-0.4946598238374698</v>
+        <v>0.4946598238374698</v>
       </c>
     </row>
     <row r="127">
@@ -2599,7 +2599,7 @@
         <v>5.30333934898738</v>
       </c>
       <c r="E127" t="n">
-        <v>0.03653090134089965</v>
+        <v>-0.03653090134089965</v>
       </c>
     </row>
     <row r="128">
@@ -2616,7 +2616,7 @@
         <v>7.021456780557162</v>
       </c>
       <c r="E128" t="n">
-        <v>0.02747817659958862</v>
+        <v>-0.02747817659958862</v>
       </c>
     </row>
     <row r="129">
@@ -2633,7 +2633,7 @@
         <v>5.154114536682522</v>
       </c>
       <c r="E129" t="n">
-        <v>0.8054459106430638</v>
+        <v>-0.8054459106430638</v>
       </c>
     </row>
     <row r="130">
@@ -2650,7 +2650,7 @@
         <v>4.498755510821064</v>
       </c>
       <c r="E130" t="n">
-        <v>0.7395466010939096</v>
+        <v>-0.7395466010939096</v>
       </c>
     </row>
     <row r="131">
@@ -2667,7 +2667,7 @@
         <v>4.843594799340205</v>
       </c>
       <c r="E131" t="n">
-        <v>0.1866471128148781</v>
+        <v>-0.1866471128148781</v>
       </c>
     </row>
     <row r="132">
@@ -2684,7 +2684,7 @@
         <v>3.987060899855996</v>
       </c>
       <c r="E132" t="n">
-        <v>0.9663221568608598</v>
+        <v>-0.9663221568608598</v>
       </c>
     </row>
     <row r="133">
@@ -2701,7 +2701,7 @@
         <v>2.694399014967422</v>
       </c>
       <c r="E133" t="n">
-        <v>1.122855255232011</v>
+        <v>-1.122855255232011</v>
       </c>
     </row>
     <row r="134">
@@ -2718,7 +2718,7 @@
         <v>3.543095604955596</v>
       </c>
       <c r="E134" t="n">
-        <v>0.4262173725415632</v>
+        <v>-0.4262173725415632</v>
       </c>
     </row>
     <row r="135">
@@ -2735,7 +2735,7 @@
         <v>3.014897121307639</v>
       </c>
       <c r="E135" t="n">
-        <v>0.2691986677396141</v>
+        <v>-0.2691986677396141</v>
       </c>
     </row>
     <row r="136">
@@ -2752,7 +2752,7 @@
         <v>4.120466681810819</v>
       </c>
       <c r="E136" t="n">
-        <v>-0.2289274792674694</v>
+        <v>0.2289274792674694</v>
       </c>
     </row>
     <row r="137">
@@ -2769,7 +2769,7 @@
         <v>3.893449748599565</v>
       </c>
       <c r="E137" t="n">
-        <v>-0.9288881857615836</v>
+        <v>0.9288881857615836</v>
       </c>
     </row>
     <row r="138">
@@ -2786,7 +2786,7 @@
         <v>5.248587573447828</v>
       </c>
       <c r="E138" t="n">
-        <v>-0.3166194291047493</v>
+        <v>0.3166194291047493</v>
       </c>
     </row>
     <row r="139">
@@ -2803,7 +2803,7 @@
         <v>3.92126649099286</v>
       </c>
       <c r="E139" t="n">
-        <v>0.7337770825794467</v>
+        <v>-0.7337770825794467</v>
       </c>
     </row>
     <row r="140">
@@ -2820,7 +2820,7 @@
         <v>4.156962474828261</v>
       </c>
       <c r="E140" t="n">
-        <v>-0.1021156809806865</v>
+        <v>0.1021156809806865</v>
       </c>
     </row>
     <row r="141">
@@ -2837,7 +2837,7 @@
         <v>4.820007904157945</v>
       </c>
       <c r="E141" t="n">
-        <v>0.2087431529682551</v>
+        <v>-0.2087431529682551</v>
       </c>
     </row>
     <row r="142">
@@ -2854,7 +2854,7 @@
         <v>3.855755505719207</v>
       </c>
       <c r="E142" t="n">
-        <v>-0.1625522657389267</v>
+        <v>0.1625522657389267</v>
       </c>
     </row>
     <row r="143">
@@ -2871,7 +2871,7 @@
         <v>4.385193439654202</v>
       </c>
       <c r="E143" t="n">
-        <v>-0.3982741338025879</v>
+        <v>0.3982741338025879</v>
       </c>
     </row>
     <row r="144">
@@ -2888,7 +2888,7 @@
         <v>5.703316949427927</v>
       </c>
       <c r="E144" t="n">
-        <v>-0.6583475256461746</v>
+        <v>0.6583475256461746</v>
       </c>
     </row>
     <row r="145">
@@ -2905,7 +2905,7 @@
         <v>4.266722292672546</v>
       </c>
       <c r="E145" t="n">
-        <v>-1.027388452577938</v>
+        <v>1.027388452577938</v>
       </c>
     </row>
     <row r="146">
@@ -2922,7 +2922,7 @@
         <v>4.547817272912461</v>
       </c>
       <c r="E146" t="n">
-        <v>-0.8655842670040865</v>
+        <v>0.8655842670040865</v>
       </c>
     </row>
     <row r="147">
@@ -2939,7 +2939,7 @@
         <v>5.020333108444674</v>
       </c>
       <c r="E147" t="n">
-        <v>-1.189706472943842</v>
+        <v>1.189706472943842</v>
       </c>
     </row>
     <row r="148">
@@ -2956,7 +2956,7 @@
         <v>5.519571001269213</v>
       </c>
       <c r="E148" t="n">
-        <v>-0.8891756797627277</v>
+        <v>0.8891756797627277</v>
       </c>
     </row>
     <row r="149">
@@ -2973,7 +2973,7 @@
         <v>4.22804436594298</v>
       </c>
       <c r="E149" t="n">
-        <v>-0.7978497612496782</v>
+        <v>0.7978497612496782</v>
       </c>
     </row>
     <row r="150">
@@ -2990,7 +2990,7 @@
         <v>3.289079573947181</v>
       </c>
       <c r="E150" t="n">
-        <v>-0.8182931789153125</v>
+        <v>0.8182931789153125</v>
       </c>
     </row>
     <row r="151">
@@ -3007,7 +3007,7 @@
         <v>4.350309536762439</v>
       </c>
       <c r="E151" t="n">
-        <v>-1.189145996248455</v>
+        <v>1.189145996248455</v>
       </c>
     </row>
     <row r="152">
@@ -3024,7 +3024,7 @@
         <v>4.843006765788845</v>
       </c>
       <c r="E152" t="n">
-        <v>-1.336140113390606</v>
+        <v>1.336140113390606</v>
       </c>
     </row>
     <row r="153">
@@ -3041,7 +3041,7 @@
         <v>4.804179215893919</v>
       </c>
       <c r="E153" t="n">
-        <v>-0.760089139795511</v>
+        <v>0.760089139795511</v>
       </c>
     </row>
     <row r="154">
@@ -3058,7 +3058,7 @@
         <v>4.871335457646478</v>
       </c>
       <c r="E154" t="n">
-        <v>-0.3947891185502517</v>
+        <v>0.3947891185502517</v>
       </c>
     </row>
     <row r="155">
@@ -3075,7 +3075,7 @@
         <v>4.411336764976275</v>
       </c>
       <c r="E155" t="n">
-        <v>-0.8587415150850566</v>
+        <v>0.8587415150850566</v>
       </c>
     </row>
     <row r="156">
@@ -3092,7 +3092,7 @@
         <v>4.604098908805144</v>
       </c>
       <c r="E156" t="n">
-        <v>-0.6924562507056682</v>
+        <v>0.6924562507056682</v>
       </c>
     </row>
     <row r="157">
@@ -3109,7 +3109,7 @@
         <v>4.599273098877139</v>
       </c>
       <c r="E157" t="n">
-        <v>-0.2038389560714116</v>
+        <v>0.2038389560714116</v>
       </c>
     </row>
     <row r="158">
@@ -3126,7 +3126,7 @@
         <v>4.343847688020986</v>
       </c>
       <c r="E158" t="n">
-        <v>-1.058491441874419</v>
+        <v>1.058491441874419</v>
       </c>
     </row>
     <row r="159">
@@ -3143,7 +3143,7 @@
         <v>5.813329125388147</v>
       </c>
       <c r="E159" t="n">
-        <v>-0.6312231834520272</v>
+        <v>0.6312231834520272</v>
       </c>
     </row>
     <row r="160">
@@ -3160,7 +3160,7 @@
         <v>5.952897751182985</v>
       </c>
       <c r="E160" t="n">
-        <v>-0.8975104727722876</v>
+        <v>0.8975104727722876</v>
       </c>
     </row>
     <row r="161">
@@ -3177,7 +3177,7 @@
         <v>4.344942874162809</v>
       </c>
       <c r="E161" t="n">
-        <v>-0.4771943255260793</v>
+        <v>0.4771943255260793</v>
       </c>
     </row>
     <row r="162">
@@ -3194,7 +3194,7 @@
         <v>5.082574096305977</v>
       </c>
       <c r="E162" t="n">
-        <v>-0.817046872799299</v>
+        <v>0.817046872799299</v>
       </c>
     </row>
     <row r="163">
@@ -3211,7 +3211,7 @@
         <v>4.529367984278831</v>
       </c>
       <c r="E163" t="n">
-        <v>-1.66196992383636</v>
+        <v>1.66196992383636</v>
       </c>
     </row>
     <row r="164">
@@ -3228,7 +3228,7 @@
         <v>5.640581986543568</v>
       </c>
       <c r="E164" t="n">
-        <v>-2.301240924280557</v>
+        <v>2.301240924280557</v>
       </c>
     </row>
     <row r="165">
@@ -3245,7 +3245,7 @@
         <v>6.338372789327269</v>
       </c>
       <c r="E165" t="n">
-        <v>-1.970820837642778</v>
+        <v>1.970820837642778</v>
       </c>
     </row>
     <row r="166">
@@ -3262,7 +3262,7 @@
         <v>5.078737604783693</v>
       </c>
       <c r="E166" t="n">
-        <v>-1.57242410987336</v>
+        <v>1.57242410987336</v>
       </c>
     </row>
     <row r="167">
@@ -3279,7 +3279,7 @@
         <v>5.964715067257329</v>
       </c>
       <c r="E167" t="n">
-        <v>-1.841603548890365</v>
+        <v>1.841603548890365</v>
       </c>
     </row>
     <row r="168">
@@ -3296,7 +3296,7 @@
         <v>5.735196360585706</v>
       </c>
       <c r="E168" t="n">
-        <v>-1.260239921764658</v>
+        <v>1.260239921764658</v>
       </c>
     </row>
     <row r="169">
@@ -3313,7 +3313,7 @@
         <v>6.473938958923769</v>
       </c>
       <c r="E169" t="n">
-        <v>-1.97070417226009</v>
+        <v>1.97070417226009</v>
       </c>
     </row>
     <row r="170">
@@ -3330,7 +3330,7 @@
         <v>7.529058223857564</v>
       </c>
       <c r="E170" t="n">
-        <v>-1.744390420757808</v>
+        <v>1.744390420757808</v>
       </c>
     </row>
     <row r="171">
@@ -3347,7 +3347,7 @@
         <v>6.750816306228175</v>
       </c>
       <c r="E171" t="n">
-        <v>-2.152754778096597</v>
+        <v>2.152754778096597</v>
       </c>
     </row>
     <row r="172">
@@ -3364,7 +3364,7 @@
         <v>5.662542565828451</v>
       </c>
       <c r="E172" t="n">
-        <v>-2.211668847672243</v>
+        <v>2.211668847672243</v>
       </c>
     </row>
     <row r="173">
@@ -3381,7 +3381,7 @@
         <v>4.603868791240572</v>
       </c>
       <c r="E173" t="n">
-        <v>-1.893483801586122</v>
+        <v>1.893483801586122</v>
       </c>
     </row>
     <row r="174">
@@ -3398,7 +3398,7 @@
         <v>4.134932723247289</v>
       </c>
       <c r="E174" t="n">
-        <v>-2.096920601560348</v>
+        <v>2.096920601560348</v>
       </c>
     </row>
     <row r="175">
@@ -3415,7 +3415,7 @@
         <v>4.315858595285953</v>
       </c>
       <c r="E175" t="n">
-        <v>-2.022075226121808</v>
+        <v>2.022075226121808</v>
       </c>
     </row>
     <row r="176">
@@ -3432,7 +3432,7 @@
         <v>4.418525589312515</v>
       </c>
       <c r="E176" t="n">
-        <v>-1.222595120809848</v>
+        <v>1.222595120809848</v>
       </c>
     </row>
     <row r="177">
@@ -3449,7 +3449,7 @@
         <v>4.78621243938987</v>
       </c>
       <c r="E177" t="n">
-        <v>-1.365219286031772</v>
+        <v>1.365219286031772</v>
       </c>
     </row>
     <row r="178">
@@ -3466,7 +3466,7 @@
         <v>5.143516646627941</v>
       </c>
       <c r="E178" t="n">
-        <v>-0.7429042403481585</v>
+        <v>0.7429042403481585</v>
       </c>
     </row>
     <row r="179">
@@ -3483,7 +3483,7 @@
         <v>5.176252350140789</v>
       </c>
       <c r="E179" t="n">
-        <v>-1.241071243386692</v>
+        <v>1.241071243386692</v>
       </c>
     </row>
     <row r="180">
@@ -3500,7 +3500,7 @@
         <v>6.010850674180727</v>
       </c>
       <c r="E180" t="n">
-        <v>-0.7967618095839946</v>
+        <v>0.7967618095839946</v>
       </c>
     </row>
     <row r="181">
@@ -3517,7 +3517,7 @@
         <v>4.874511154015846</v>
       </c>
       <c r="E181" t="n">
-        <v>0.07018979672125525</v>
+        <v>-0.07018979672125525</v>
       </c>
     </row>
     <row r="182">
@@ -3534,7 +3534,7 @@
         <v>7.544548042761498</v>
       </c>
       <c r="E182" t="n">
-        <v>-1.244475036849238</v>
+        <v>1.244475036849238</v>
       </c>
     </row>
     <row r="183">
@@ -3551,7 +3551,7 @@
         <v>7.323981278705968</v>
       </c>
       <c r="E183" t="n">
-        <v>-1.500390494731853</v>
+        <v>1.500390494731853</v>
       </c>
     </row>
     <row r="184">
@@ -3568,7 +3568,7 @@
         <v>5.582621659704566</v>
       </c>
       <c r="E184" t="n">
-        <v>-0.9967449810151585</v>
+        <v>0.9967449810151585</v>
       </c>
     </row>
     <row r="185">
@@ -3585,7 +3585,7 @@
         <v>4.346698617945521</v>
       </c>
       <c r="E185" t="n">
-        <v>-0.9718638036260305</v>
+        <v>0.9718638036260305</v>
       </c>
     </row>
     <row r="186">
@@ -3602,7 +3602,7 @@
         <v>4.63103367272139</v>
       </c>
       <c r="E186" t="n">
-        <v>-0.6470302248825988</v>
+        <v>0.6470302248825988</v>
       </c>
     </row>
     <row r="187">
@@ -3619,7 +3619,7 @@
         <v>4.468220340071008</v>
       </c>
       <c r="E187" t="n">
-        <v>-0.8802532563663026</v>
+        <v>0.8802532563663026</v>
       </c>
     </row>
     <row r="188">
@@ -3636,7 +3636,7 @@
         <v>4.978619992369852</v>
       </c>
       <c r="E188" t="n">
-        <v>-0.7178464212632605</v>
+        <v>0.7178464212632605</v>
       </c>
     </row>
     <row r="189">
@@ -3653,7 +3653,7 @@
         <v>5.185140905240265</v>
       </c>
       <c r="E189" t="n">
-        <v>-0.7049159090614943</v>
+        <v>0.7049159090614943</v>
       </c>
     </row>
     <row r="190">
@@ -3670,7 +3670,7 @@
         <v>4.521556308546418</v>
       </c>
       <c r="E190" t="n">
-        <v>0.005265519278722763</v>
+        <v>-0.005265519278722763</v>
       </c>
     </row>
     <row r="191">
@@ -3687,7 +3687,7 @@
         <v>3.589616579473113</v>
       </c>
       <c r="E191" t="n">
-        <v>0.1389360709094243</v>
+        <v>-0.1389360709094243</v>
       </c>
     </row>
     <row r="192">
@@ -3704,7 +3704,7 @@
         <v>2.343597172689355</v>
       </c>
       <c r="E192" t="n">
-        <v>0.2988200736427009</v>
+        <v>-0.2988200736427009</v>
       </c>
     </row>
     <row r="193">
@@ -3721,7 +3721,7 @@
         <v>2.553163877465106</v>
       </c>
       <c r="E193" t="n">
-        <v>0.04168555334774116</v>
+        <v>-0.04168555334774116</v>
       </c>
     </row>
     <row r="194">
@@ -3738,7 +3738,7 @@
         <v>3.836755381978047</v>
       </c>
       <c r="E194" t="n">
-        <v>-0.2213615664390334</v>
+        <v>0.2213615664390334</v>
       </c>
     </row>
     <row r="195">
@@ -3755,7 +3755,7 @@
         <v>4.206000501263961</v>
       </c>
       <c r="E195" t="n">
-        <v>-0.4204695508078875</v>
+        <v>0.4204695508078875</v>
       </c>
     </row>
     <row r="196">
@@ -3772,7 +3772,7 @@
         <v>3.039100466684348</v>
       </c>
       <c r="E196" t="n">
-        <v>-0.1564132970003298</v>
+        <v>0.1564132970003298</v>
       </c>
     </row>
     <row r="197">
@@ -3789,7 +3789,7 @@
         <v>3.6078941835509</v>
       </c>
       <c r="E197" t="n">
-        <v>-0.3580175643153733</v>
+        <v>0.3580175643153733</v>
       </c>
     </row>
     <row r="198">
@@ -3806,7 +3806,7 @@
         <v>4.015829401484915</v>
       </c>
       <c r="E198" t="n">
-        <v>-0.1575229037227786</v>
+        <v>0.1575229037227786</v>
       </c>
     </row>
     <row r="199">
@@ -3823,7 +3823,7 @@
         <v>2.750198069837801</v>
       </c>
       <c r="E199" t="n">
-        <v>0.9594476903050984</v>
+        <v>-0.9594476903050984</v>
       </c>
     </row>
     <row r="200">
@@ -3840,7 +3840,7 @@
         <v>2.961768604183987</v>
       </c>
       <c r="E200" t="n">
-        <v>1.292346087342487</v>
+        <v>-1.292346087342487</v>
       </c>
     </row>
     <row r="201">
@@ -3857,7 +3857,7 @@
         <v>3.320861370530626</v>
       </c>
       <c r="E201" t="n">
-        <v>0.9488639162623151</v>
+        <v>-0.9488639162623151</v>
       </c>
     </row>
     <row r="202">
@@ -3874,7 +3874,7 @@
         <v>2.192165200400721</v>
       </c>
       <c r="E202" t="n">
-        <v>1.45749675381823</v>
+        <v>-1.45749675381823</v>
       </c>
     </row>
     <row r="203">
@@ -3891,7 +3891,7 @@
         <v>3.046723887923608</v>
       </c>
       <c r="E203" t="n">
-        <v>1.048789773784427</v>
+        <v>-1.048789773784427</v>
       </c>
     </row>
     <row r="204">
@@ -3908,7 +3908,7 @@
         <v>4.283665513345221</v>
       </c>
       <c r="E204" t="n">
-        <v>-0.1666295228637367</v>
+        <v>0.1666295228637367</v>
       </c>
     </row>
     <row r="205">
@@ -3925,7 +3925,7 @@
         <v>5.421577244110583</v>
       </c>
       <c r="E205" t="n">
-        <v>-0.6769485215879936</v>
+        <v>0.6769485215879936</v>
       </c>
     </row>
     <row r="206">
@@ -3942,7 +3942,7 @@
         <v>6.468276240199284</v>
       </c>
       <c r="E206" t="n">
-        <v>-1.575250586905934</v>
+        <v>1.575250586905934</v>
       </c>
     </row>
     <row r="207">
@@ -3959,7 +3959,7 @@
         <v>4.837707683607935</v>
       </c>
       <c r="E207" t="n">
-        <v>-1.552100840188023</v>
+        <v>1.552100840188023</v>
       </c>
     </row>
     <row r="208">
@@ -3976,7 +3976,7 @@
         <v>3.968487718137356</v>
       </c>
       <c r="E208" t="n">
-        <v>-1.336645677203705</v>
+        <v>1.336645677203705</v>
       </c>
     </row>
     <row r="209">
@@ -3993,7 +3993,7 @@
         <v>4.127314346758526</v>
       </c>
       <c r="E209" t="n">
-        <v>-0.2740912587091349</v>
+        <v>0.2740912587091349</v>
       </c>
     </row>
     <row r="210">
@@ -4010,7 +4010,7 @@
         <v>4.509526220851713</v>
       </c>
       <c r="E210" t="n">
-        <v>-0.06509932271529983</v>
+        <v>0.06509932271529983</v>
       </c>
     </row>
     <row r="211">
@@ -4027,7 +4027,7 @@
         <v>4.90950816585681</v>
       </c>
       <c r="E211" t="n">
-        <v>-0.1721851416099209</v>
+        <v>0.1721851416099209</v>
       </c>
     </row>
     <row r="212">
@@ -4044,7 +4044,7 @@
         <v>7.72854421346858</v>
       </c>
       <c r="E212" t="n">
-        <v>0.2886755443311566</v>
+        <v>-0.2886755443311566</v>
       </c>
     </row>
     <row r="213">
@@ -4061,7 +4061,7 @@
         <v>7.717889435849886</v>
       </c>
       <c r="E213" t="n">
-        <v>-0.9173651727710102</v>
+        <v>0.9173651727710102</v>
       </c>
     </row>
     <row r="214">
@@ -4078,7 +4078,7 @@
         <v>7.643674175215222</v>
       </c>
       <c r="E214" t="n">
-        <v>-0.6713340712265765</v>
+        <v>0.6713340712265765</v>
       </c>
     </row>
     <row r="215">
@@ -4095,7 +4095,7 @@
         <v>7.282316347418433</v>
       </c>
       <c r="E215" t="n">
-        <v>-0.17522943241433</v>
+        <v>0.17522943241433</v>
       </c>
     </row>
     <row r="216">
@@ -4112,7 +4112,7 @@
         <v>7.332768795595162</v>
       </c>
       <c r="E216" t="n">
-        <v>-0.9328958905761962</v>
+        <v>0.9328958905761962</v>
       </c>
     </row>
     <row r="217">
@@ -4129,7 +4129,7 @@
         <v>5.932445288425672</v>
       </c>
       <c r="E217" t="n">
-        <v>-0.2051862153659343</v>
+        <v>0.2051862153659343</v>
       </c>
     </row>
     <row r="218">
@@ -4146,7 +4146,7 @@
         <v>6.010401595556276</v>
       </c>
       <c r="E218" t="n">
-        <v>0.00078250731527163</v>
+        <v>-0.00078250731527163</v>
       </c>
     </row>
     <row r="219">
@@ -4163,7 +4163,7 @@
         <v>4.966410011098013</v>
       </c>
       <c r="E219" t="n">
-        <v>-0.2186491859798245</v>
+        <v>0.2186491859798245</v>
       </c>
     </row>
     <row r="220">
@@ -4180,7 +4180,7 @@
         <v>4.432017156679582</v>
       </c>
       <c r="E220" t="n">
-        <v>0.144526399342471</v>
+        <v>-0.144526399342471</v>
       </c>
     </row>
     <row r="221">
@@ -4197,7 +4197,7 @@
         <v>3.391902005171922</v>
       </c>
       <c r="E221" t="n">
-        <v>1.324601499374905</v>
+        <v>-1.324601499374905</v>
       </c>
     </row>
     <row r="222">
@@ -4214,7 +4214,7 @@
         <v>3.598471460099544</v>
       </c>
       <c r="E222" t="n">
-        <v>1.245078179363659</v>
+        <v>-1.245078179363659</v>
       </c>
     </row>
     <row r="223">
@@ -4231,7 +4231,7 @@
         <v>5.61304829796143</v>
       </c>
       <c r="E223" t="n">
-        <v>1.211139539354333</v>
+        <v>-1.211139539354333</v>
       </c>
     </row>
     <row r="224">
@@ -4248,7 +4248,7 @@
         <v>3.709771922953554</v>
       </c>
       <c r="E224" t="n">
-        <v>0.8080010337785839</v>
+        <v>-0.8080010337785839</v>
       </c>
     </row>
     <row r="225">
@@ -4265,7 +4265,7 @@
         <v>4.66294931634327</v>
       </c>
       <c r="E225" t="n">
-        <v>0.2520698237097534</v>
+        <v>-0.2520698237097534</v>
       </c>
     </row>
     <row r="226">
@@ -4282,7 +4282,7 @@
         <v>3.009964861949143</v>
       </c>
       <c r="E226" t="n">
-        <v>0.6571876753629198</v>
+        <v>-0.6571876753629198</v>
       </c>
     </row>
     <row r="227">
@@ -4299,7 +4299,7 @@
         <v>3.227584678104821</v>
       </c>
       <c r="E227" t="n">
-        <v>0.1179511923679328</v>
+        <v>-0.1179511923679328</v>
       </c>
     </row>
     <row r="228">
@@ -4316,7 +4316,7 @@
         <v>4.497351946067726</v>
       </c>
       <c r="E228" t="n">
-        <v>0.1401136201209159</v>
+        <v>-0.1401136201209159</v>
       </c>
     </row>
     <row r="229">
@@ -4333,7 +4333,7 @@
         <v>4.677045950091158</v>
       </c>
       <c r="E229" t="n">
-        <v>-0.1307256427715977</v>
+        <v>0.1307256427715977</v>
       </c>
     </row>
     <row r="230">
@@ -4350,7 +4350,7 @@
         <v>3.62119188681142</v>
       </c>
       <c r="E230" t="n">
-        <v>0.1395676572903009</v>
+        <v>-0.1395676572903009</v>
       </c>
     </row>
     <row r="231">
@@ -4367,7 +4367,7 @@
         <v>3.208606118080461</v>
       </c>
       <c r="E231" t="n">
-        <v>0.2972867996200526</v>
+        <v>-0.2972867996200526</v>
       </c>
     </row>
     <row r="232">
@@ -4384,7 +4384,7 @@
         <v>3.89890553431807</v>
       </c>
       <c r="E232" t="n">
-        <v>0.8058429317084101</v>
+        <v>-0.8058429317084101</v>
       </c>
     </row>
     <row r="233">
@@ -4401,7 +4401,7 @@
         <v>3.572633071806935</v>
       </c>
       <c r="E233" t="n">
-        <v>0.4296727298215499</v>
+        <v>-0.4296727298215499</v>
       </c>
     </row>
     <row r="234">
@@ -4418,7 +4418,7 @@
         <v>4.114418872622053</v>
       </c>
       <c r="E234" t="n">
-        <v>0.230190164157678</v>
+        <v>-0.230190164157678</v>
       </c>
     </row>
     <row r="235">
@@ -4435,7 +4435,7 @@
         <v>4.562139290393978</v>
       </c>
       <c r="E235" t="n">
-        <v>-0.3172401876023176</v>
+        <v>0.3172401876023176</v>
       </c>
     </row>
     <row r="236">
@@ -4452,7 +4452,7 @@
         <v>4.202864907388613</v>
       </c>
       <c r="E236" t="n">
-        <v>-0.5098373570571861</v>
+        <v>0.5098373570571861</v>
       </c>
     </row>
     <row r="237">
@@ -4469,7 +4469,7 @@
         <v>6.105166702472856</v>
       </c>
       <c r="E237" t="n">
-        <v>-0.2429939659889229</v>
+        <v>0.2429939659889229</v>
       </c>
     </row>
     <row r="238">
@@ -4486,7 +4486,7 @@
         <v>6.056053539999334</v>
       </c>
       <c r="E238" t="n">
-        <v>0.1890063695406141</v>
+        <v>-0.1890063695406141</v>
       </c>
     </row>
     <row r="239">
@@ -4503,7 +4503,7 @@
         <v>4.204720979270228</v>
       </c>
       <c r="E239" t="n">
-        <v>-0.3230735781517899</v>
+        <v>0.3230735781517899</v>
       </c>
     </row>
     <row r="240">
@@ -4520,7 +4520,7 @@
         <v>4.341889563556775</v>
       </c>
       <c r="E240" t="n">
-        <v>0.1790182554680726</v>
+        <v>-0.1790182554680726</v>
       </c>
     </row>
     <row r="241">
@@ -4537,7 +4537,7 @@
         <v>3.564033201550127</v>
       </c>
       <c r="E241" t="n">
-        <v>0.8712491987900033</v>
+        <v>-0.8712491987900033</v>
       </c>
     </row>
     <row r="242">
@@ -4554,7 +4554,7 @@
         <v>4.489796597523842</v>
       </c>
       <c r="E242" t="n">
-        <v>0.9741162419785532</v>
+        <v>-0.9741162419785532</v>
       </c>
     </row>
     <row r="243">
@@ -4571,7 +4571,7 @@
         <v>3.371073452839728</v>
       </c>
       <c r="E243" t="n">
-        <v>1.836200200258032</v>
+        <v>-1.836200200258032</v>
       </c>
     </row>
     <row r="244">
@@ -4588,7 +4588,7 @@
         <v>3.792882964458096</v>
       </c>
       <c r="E244" t="n">
-        <v>1.184150680874533</v>
+        <v>-1.184150680874533</v>
       </c>
     </row>
     <row r="245">
@@ -4605,7 +4605,7 @@
         <v>4.796216124257996</v>
       </c>
       <c r="E245" t="n">
-        <v>0.3698485558096252</v>
+        <v>-0.3698485558096252</v>
       </c>
     </row>
     <row r="246">
@@ -4622,7 +4622,7 @@
         <v>6.019967374528983</v>
       </c>
       <c r="E246" t="n">
-        <v>-0.6185780627411219</v>
+        <v>0.6185780627411219</v>
       </c>
     </row>
     <row r="247">
@@ -4639,7 +4639,7 @@
         <v>4.369508143408408</v>
       </c>
       <c r="E247" t="n">
-        <v>0.253526158749839</v>
+        <v>-0.253526158749839</v>
       </c>
     </row>
     <row r="248">
@@ -4656,7 +4656,7 @@
         <v>4.098383813033593</v>
       </c>
       <c r="E248" t="n">
-        <v>0.5655150217567844</v>
+        <v>-0.5655150217567844</v>
       </c>
     </row>
     <row r="249">
@@ -4673,7 +4673,7 @@
         <v>3.961052343376871</v>
       </c>
       <c r="E249" t="n">
-        <v>0.4612009720379002</v>
+        <v>-0.4612009720379002</v>
       </c>
     </row>
     <row r="250">
@@ -4690,7 +4690,7 @@
         <v>3.644317083893736</v>
       </c>
       <c r="E250" t="n">
-        <v>0.5479308879473357</v>
+        <v>-0.5479308879473357</v>
       </c>
     </row>
     <row r="251">
@@ -4707,7 +4707,7 @@
         <v>5.826269108245673</v>
       </c>
       <c r="E251" t="n">
-        <v>-0.1191060883616597</v>
+        <v>0.1191060883616597</v>
       </c>
     </row>
     <row r="252">
@@ -4724,7 +4724,7 @@
         <v>5.335032861805519</v>
       </c>
       <c r="E252" t="n">
-        <v>1.188367759619645</v>
+        <v>-1.188367759619645</v>
       </c>
     </row>
     <row r="253">
@@ -4741,7 +4741,7 @@
         <v>4.104349550878228</v>
       </c>
       <c r="E253" t="n">
-        <v>1.099098250006399</v>
+        <v>-1.099098250006399</v>
       </c>
     </row>
     <row r="254">
@@ -4758,7 +4758,7 @@
         <v>5.093268607130714</v>
       </c>
       <c r="E254" t="n">
-        <v>1.011190226564684</v>
+        <v>-1.011190226564684</v>
       </c>
     </row>
     <row r="255">
@@ -4775,7 +4775,7 @@
         <v>6.65150558740764</v>
       </c>
       <c r="E255" t="n">
-        <v>1.260461605506277</v>
+        <v>-1.260461605506277</v>
       </c>
     </row>
     <row r="256">
@@ -4792,7 +4792,7 @@
         <v>6.882116017581236</v>
       </c>
       <c r="E256" t="n">
-        <v>1.347427694213655</v>
+        <v>-1.347427694213655</v>
       </c>
     </row>
     <row r="257">
@@ -4809,7 +4809,7 @@
         <v>4.971610307801852</v>
       </c>
       <c r="E257" t="n">
-        <v>1.287069852513886</v>
+        <v>-1.287069852513886</v>
       </c>
     </row>
     <row r="258">
@@ -4826,7 +4826,7 @@
         <v>4.78443860583058</v>
       </c>
       <c r="E258" t="n">
-        <v>0.6989943688891138</v>
+        <v>-0.6989943688891138</v>
       </c>
     </row>
     <row r="259">
@@ -4843,7 +4843,7 @@
         <v>5.849044710097617</v>
       </c>
       <c r="E259" t="n">
-        <v>0.8553429188037693</v>
+        <v>-0.8553429188037693</v>
       </c>
     </row>
     <row r="260">
@@ -4860,7 +4860,7 @@
         <v>4.561652329428824</v>
       </c>
       <c r="E260" t="n">
-        <v>1.73593148662531</v>
+        <v>-1.73593148662531</v>
       </c>
     </row>
     <row r="261">
@@ -4877,7 +4877,7 @@
         <v>4.704434608780404</v>
       </c>
       <c r="E261" t="n">
-        <v>2.216400398488386</v>
+        <v>-2.216400398488386</v>
       </c>
     </row>
     <row r="262">
@@ -4894,7 +4894,7 @@
         <v>4.986722512117795</v>
       </c>
       <c r="E262" t="n">
-        <v>2.764038281391812</v>
+        <v>-2.764038281391812</v>
       </c>
     </row>
     <row r="263">
@@ -4911,7 +4911,7 @@
         <v>4.276025104003066</v>
       </c>
       <c r="E263" t="n">
-        <v>2.127679929444998</v>
+        <v>-2.127679929444998</v>
       </c>
     </row>
     <row r="264">
@@ -4928,7 +4928,7 @@
         <v>4.69560944751198</v>
       </c>
       <c r="E264" t="n">
-        <v>1.323015644376689</v>
+        <v>-1.323015644376689</v>
       </c>
     </row>
     <row r="265">
@@ -4945,7 +4945,7 @@
         <v>2.167368884994072</v>
       </c>
       <c r="E265" t="n">
-        <v>1.081220197162594</v>
+        <v>-1.081220197162594</v>
       </c>
     </row>
     <row r="266">
@@ -4962,7 +4962,7 @@
         <v>2.239147456320685</v>
       </c>
       <c r="E266" t="n">
-        <v>0.9673369436597579</v>
+        <v>-0.9673369436597579</v>
       </c>
     </row>
     <row r="267">
@@ -4979,7 +4979,7 @@
         <v>2.682853210195256</v>
       </c>
       <c r="E267" t="n">
-        <v>1.416998970269281</v>
+        <v>-1.416998970269281</v>
       </c>
     </row>
     <row r="268">
@@ -4996,7 +4996,7 @@
         <v>2.866811029131801</v>
       </c>
       <c r="E268" t="n">
-        <v>0.3353293047933095</v>
+        <v>-0.3353293047933095</v>
       </c>
     </row>
     <row r="269">
@@ -5013,7 +5013,7 @@
         <v>4.663360750495595</v>
       </c>
       <c r="E269" t="n">
-        <v>1.098690751539063</v>
+        <v>-1.098690751539063</v>
       </c>
     </row>
     <row r="270">
@@ -5030,7 +5030,7 @@
         <v>3.743379570662131</v>
       </c>
       <c r="E270" t="n">
-        <v>0.8696120899051754</v>
+        <v>-0.8696120899051754</v>
       </c>
     </row>
     <row r="271">
@@ -5047,7 +5047,7 @@
         <v>4.030250354461009</v>
       </c>
       <c r="E271" t="n">
-        <v>0.5288960722740139</v>
+        <v>-0.5288960722740139</v>
       </c>
     </row>
     <row r="272">
@@ -5064,7 +5064,7 @@
         <v>4.903691797611915</v>
       </c>
       <c r="E272" t="n">
-        <v>-0.07573549428207471</v>
+        <v>0.07573549428207471</v>
       </c>
     </row>
     <row r="273">
@@ -5081,7 +5081,7 @@
         <v>6.846467905785794</v>
       </c>
       <c r="E273" t="n">
-        <v>-0.9396842047830454</v>
+        <v>0.9396842047830454</v>
       </c>
     </row>
     <row r="274">
@@ -5098,7 +5098,7 @@
         <v>5.220303051251744</v>
       </c>
       <c r="E274" t="n">
-        <v>-0.3803860136946202</v>
+        <v>0.3803860136946202</v>
       </c>
     </row>
     <row r="275">
@@ -5115,7 +5115,7 @@
         <v>6.424464229946886</v>
       </c>
       <c r="E275" t="n">
-        <v>-0.2912448638105616</v>
+        <v>0.2912448638105616</v>
       </c>
     </row>
     <row r="276">
@@ -5132,7 +5132,7 @@
         <v>6.663233591350661</v>
       </c>
       <c r="E276" t="n">
-        <v>-0.9339141172384604</v>
+        <v>0.9339141172384604</v>
       </c>
     </row>
     <row r="277">
@@ -5149,7 +5149,7 @@
         <v>6.063128553513424</v>
       </c>
       <c r="E277" t="n">
-        <v>-1.494101807835399</v>
+        <v>1.494101807835399</v>
       </c>
     </row>
     <row r="278">
@@ -5166,7 +5166,7 @@
         <v>6.658256181647614</v>
       </c>
       <c r="E278" t="n">
-        <v>-1.473401247427274</v>
+        <v>1.473401247427274</v>
       </c>
     </row>
     <row r="279">
@@ -5183,7 +5183,7 @@
         <v>6.33364169010788</v>
       </c>
       <c r="E279" t="n">
-        <v>-0.3966366938202324</v>
+        <v>0.3966366938202324</v>
       </c>
     </row>
     <row r="280">
@@ -5200,7 +5200,7 @@
         <v>5.864951192682233</v>
       </c>
       <c r="E280" t="n">
-        <v>-0.4811625253731098</v>
+        <v>0.4811625253731098</v>
       </c>
     </row>
     <row r="281">
@@ -5217,7 +5217,7 @@
         <v>6.444729021537981</v>
       </c>
       <c r="E281" t="n">
-        <v>-1.211247430886555</v>
+        <v>1.211247430886555</v>
       </c>
     </row>
     <row r="282">
@@ -5234,7 +5234,7 @@
         <v>6.207997197098948</v>
       </c>
       <c r="E282" t="n">
-        <v>-1.180484521527308</v>
+        <v>1.180484521527308</v>
       </c>
     </row>
     <row r="283">
@@ -5251,7 +5251,7 @@
         <v>6.475713167332053</v>
       </c>
       <c r="E283" t="n">
-        <v>-1.168048514878063</v>
+        <v>1.168048514878063</v>
       </c>
     </row>
     <row r="284">
@@ -5268,7 +5268,7 @@
         <v>7.773265095539084</v>
       </c>
       <c r="E284" t="n">
-        <v>-2.437545604629161</v>
+        <v>2.437545604629161</v>
       </c>
     </row>
     <row r="285">
@@ -5285,7 +5285,7 @@
         <v>8.876424164500481</v>
       </c>
       <c r="E285" t="n">
-        <v>-2.143128948488267</v>
+        <v>2.143128948488267</v>
       </c>
     </row>
     <row r="286">
@@ -5302,7 +5302,7 @@
         <v>7.310997334673755</v>
       </c>
       <c r="E286" t="n">
-        <v>-1.981026157638091</v>
+        <v>1.981026157638091</v>
       </c>
     </row>
     <row r="287">
@@ -5319,7 +5319,7 @@
         <v>8.795845836797371</v>
       </c>
       <c r="E287" t="n">
-        <v>-1.350754445044316</v>
+        <v>1.350754445044316</v>
       </c>
     </row>
     <row r="288">
@@ -5336,7 +5336,7 @@
         <v>6.059868106696133</v>
       </c>
       <c r="E288" t="n">
-        <v>-0.1952167762959292</v>
+        <v>0.1952167762959292</v>
       </c>
     </row>
     <row r="289">
@@ -5353,7 +5353,7 @@
         <v>5.758555017587923</v>
       </c>
       <c r="E289" t="n">
-        <v>0.4256369328719511</v>
+        <v>-0.4256369328719511</v>
       </c>
     </row>
     <row r="290">
@@ -5370,7 +5370,7 @@
         <v>6.495578348808634</v>
       </c>
       <c r="E290" t="n">
-        <v>0.227210173907503</v>
+        <v>-0.227210173907503</v>
       </c>
     </row>
     <row r="291">
@@ -5387,7 +5387,7 @@
         <v>7.001799664603391</v>
       </c>
       <c r="E291" t="n">
-        <v>-0.3873008385593941</v>
+        <v>0.3873008385593941</v>
       </c>
     </row>
     <row r="292">
@@ -5404,7 +5404,7 @@
         <v>5.687282304041414</v>
       </c>
       <c r="E292" t="n">
-        <v>1.023115796963113</v>
+        <v>-1.023115796963113</v>
       </c>
     </row>
     <row r="293">
@@ -5421,7 +5421,7 @@
         <v>5.670442364451841</v>
       </c>
       <c r="E293" t="n">
-        <v>0.9187792124950924</v>
+        <v>-0.9187792124950924</v>
       </c>
     </row>
     <row r="294">
@@ -5438,7 +5438,7 @@
         <v>5.449994284894798</v>
       </c>
       <c r="E294" t="n">
-        <v>0.8043534587148446</v>
+        <v>-0.8043534587148446</v>
       </c>
     </row>
     <row r="295">
@@ -5455,7 +5455,7 @@
         <v>5.244008899620956</v>
       </c>
       <c r="E295" t="n">
-        <v>0.6849967639857724</v>
+        <v>-0.6849967639857724</v>
       </c>
     </row>
     <row r="296">
@@ -5472,7 +5472,7 @@
         <v>6.26880829859576</v>
       </c>
       <c r="E296" t="n">
-        <v>0.6988172936558872</v>
+        <v>-0.6988172936558872</v>
       </c>
     </row>
     <row r="297">
@@ -5489,7 +5489,7 @@
         <v>6.672408560404324</v>
       </c>
       <c r="E297" t="n">
-        <v>0.5299487489940926</v>
+        <v>-0.5299487489940926</v>
       </c>
     </row>
     <row r="298">
@@ -5506,7 +5506,7 @@
         <v>6.210848746532528</v>
       </c>
       <c r="E298" t="n">
-        <v>0.1567342976075441</v>
+        <v>-0.1567342976075441</v>
       </c>
     </row>
     <row r="299">
@@ -5523,7 +5523,7 @@
         <v>7.258025586416071</v>
       </c>
       <c r="E299" t="n">
-        <v>-0.1528557150802854</v>
+        <v>0.1528557150802854</v>
       </c>
     </row>
     <row r="300">
@@ -5540,7 +5540,7 @@
         <v>7.39416298145342</v>
       </c>
       <c r="E300" t="n">
-        <v>-0.1498931439141611</v>
+        <v>0.1498931439141611</v>
       </c>
     </row>
     <row r="301">
@@ -5557,7 +5557,7 @@
         <v>8.058080389385397</v>
       </c>
       <c r="E301" t="n">
-        <v>-0.4170266147555308</v>
+        <v>0.4170266147555308</v>
       </c>
     </row>
     <row r="302">
@@ -5574,7 +5574,7 @@
         <v>8.445891187916249</v>
       </c>
       <c r="E302" t="n">
-        <v>-0.7382292144663971</v>
+        <v>0.7382292144663971</v>
       </c>
     </row>
     <row r="303">
@@ -5591,7 +5591,7 @@
         <v>7.3127740289016</v>
       </c>
       <c r="E303" t="n">
-        <v>-0.5841689485922128</v>
+        <v>0.5841689485922128</v>
       </c>
     </row>
     <row r="304">
@@ -5608,7 +5608,7 @@
         <v>6.836206747941919</v>
       </c>
       <c r="E304" t="n">
-        <v>-0.641400880694853</v>
+        <v>0.641400880694853</v>
       </c>
     </row>
     <row r="305">
@@ -5625,7 +5625,7 @@
         <v>7.149380423098592</v>
       </c>
       <c r="E305" t="n">
-        <v>0.2379264309130527</v>
+        <v>-0.2379264309130527</v>
       </c>
     </row>
     <row r="306">
@@ -5642,7 +5642,7 @@
         <v>8.28687569656342</v>
       </c>
       <c r="E306" t="n">
-        <v>-1.193679473533838</v>
+        <v>1.193679473533838</v>
       </c>
     </row>
     <row r="307">
@@ -5659,7 +5659,7 @@
         <v>7.694035465444848</v>
       </c>
       <c r="E307" t="n">
-        <v>-0.458997026933913</v>
+        <v>0.458997026933913</v>
       </c>
     </row>
     <row r="308">
@@ -5676,7 +5676,7 @@
         <v>7.301481440500508</v>
       </c>
       <c r="E308" t="n">
-        <v>0.259942962374339</v>
+        <v>-0.259942962374339</v>
       </c>
     </row>
     <row r="309">
@@ -5693,7 +5693,7 @@
         <v>8.826025751939241</v>
       </c>
       <c r="E309" t="n">
-        <v>-0.8695413501028781</v>
+        <v>0.8695413501028781</v>
       </c>
     </row>
     <row r="310">
@@ -5710,7 +5710,7 @@
         <v>7.97086304801469</v>
       </c>
       <c r="E310" t="n">
-        <v>-0.9352706535545323</v>
+        <v>0.9352706535545323</v>
       </c>
     </row>
     <row r="311">
@@ -5727,7 +5727,7 @@
         <v>8.349244942021102</v>
       </c>
       <c r="E311" t="n">
-        <v>-1.007473274620525</v>
+        <v>1.007473274620525</v>
       </c>
     </row>
     <row r="312">
@@ -5744,7 +5744,7 @@
         <v>8.273451351946044</v>
       </c>
       <c r="E312" t="n">
-        <v>-1.617290582192005</v>
+        <v>1.617290582192005</v>
       </c>
     </row>
     <row r="313">
@@ -5761,7 +5761,7 @@
         <v>8.100276480027322</v>
       </c>
       <c r="E313" t="n">
-        <v>-1.813714051152299</v>
+        <v>1.813714051152299</v>
       </c>
     </row>
     <row r="314">
@@ -5778,7 +5778,7 @@
         <v>9.196723908980559</v>
       </c>
       <c r="E314" t="n">
-        <v>-2.159843663537732</v>
+        <v>2.159843663537732</v>
       </c>
     </row>
     <row r="315">
@@ -5795,7 +5795,7 @@
         <v>9.016662222929858</v>
       </c>
       <c r="E315" t="n">
-        <v>-0.948125932614623</v>
+        <v>0.948125932614623</v>
       </c>
     </row>
     <row r="316">
@@ -5812,7 +5812,7 @@
         <v>9.003236819649294</v>
       </c>
       <c r="E316" t="n">
-        <v>-0.3282895255329557</v>
+        <v>0.3282895255329557</v>
       </c>
     </row>
     <row r="317">
@@ -5829,7 +5829,7 @@
         <v>9.274509730594529</v>
       </c>
       <c r="E317" t="n">
-        <v>0.3867769933208365</v>
+        <v>-0.3867769933208365</v>
       </c>
     </row>
     <row r="318">
@@ -5846,7 +5846,7 @@
         <v>8.479696523450347</v>
       </c>
       <c r="E318" t="n">
-        <v>0.7166505839919601</v>
+        <v>-0.7166505839919601</v>
       </c>
     </row>
     <row r="319">
@@ -5863,7 +5863,7 @@
         <v>8.946591214300604</v>
       </c>
       <c r="E319" t="n">
-        <v>0.02536856039348478</v>
+        <v>-0.02536856039348478</v>
       </c>
     </row>
     <row r="320">
@@ -5880,7 +5880,7 @@
         <v>8.346350576144161</v>
       </c>
       <c r="E320" t="n">
-        <v>-0.2550113635110023</v>
+        <v>0.2550113635110023</v>
       </c>
     </row>
     <row r="321">
@@ -5897,7 +5897,7 @@
         <v>8.22149985958697</v>
       </c>
       <c r="E321" t="n">
-        <v>0.03724557435229414</v>
+        <v>-0.03724557435229414</v>
       </c>
     </row>
     <row r="322">
@@ -5914,7 +5914,7 @@
         <v>8.18757105491375</v>
       </c>
       <c r="E322" t="n">
-        <v>-0.6131394000176362</v>
+        <v>0.6131394000176362</v>
       </c>
     </row>
     <row r="323">
@@ -5931,7 +5931,7 @@
         <v>7.904953819186393</v>
       </c>
       <c r="E323" t="n">
-        <v>-0.1553097933831893</v>
+        <v>0.1553097933831893</v>
       </c>
     </row>
     <row r="324">
@@ -5948,7 +5948,7 @@
         <v>8.345872130611246</v>
       </c>
       <c r="E324" t="n">
-        <v>-0.2616479905653648</v>
+        <v>0.2616479905653648</v>
       </c>
     </row>
     <row r="325">
@@ -5965,7 +5965,7 @@
         <v>7.519622513053625</v>
       </c>
       <c r="E325" t="n">
-        <v>-0.424922976001028</v>
+        <v>0.424922976001028</v>
       </c>
     </row>
     <row r="326">
@@ -5982,7 +5982,7 @@
         <v>9.118024156577359</v>
       </c>
       <c r="E326" t="n">
-        <v>0.00688234779844521</v>
+        <v>-0.00688234779844521</v>
       </c>
     </row>
     <row r="327">
@@ -5999,7 +5999,7 @@
         <v>7.678034435090395</v>
       </c>
       <c r="E327" t="n">
-        <v>0.2406009943069609</v>
+        <v>-0.2406009943069609</v>
       </c>
     </row>
     <row r="328">
@@ -6016,7 +6016,7 @@
         <v>6.693895973201353</v>
       </c>
       <c r="E328" t="n">
-        <v>0.01807105552388855</v>
+        <v>-0.01807105552388855</v>
       </c>
     </row>
     <row r="329">
@@ -6033,7 +6033,7 @@
         <v>7.619492790468297</v>
       </c>
       <c r="E329" t="n">
-        <v>0.6279581160784327</v>
+        <v>-0.6279581160784327</v>
       </c>
     </row>
     <row r="330">
@@ -6050,7 +6050,7 @@
         <v>8.507618003063909</v>
       </c>
       <c r="E330" t="n">
-        <v>-0.02622353905114139</v>
+        <v>0.02622353905114139</v>
       </c>
     </row>
     <row r="331">
@@ -6067,7 +6067,7 @@
         <v>8.601934444180706</v>
       </c>
       <c r="E331" t="n">
-        <v>0.3025493274989017</v>
+        <v>-0.3025493274989017</v>
       </c>
     </row>
     <row r="332">
@@ -6084,7 +6084,7 @@
         <v>8.656267031756503</v>
       </c>
       <c r="E332" t="n">
-        <v>0.5756844132370738</v>
+        <v>-0.5756844132370738</v>
       </c>
     </row>
     <row r="333">
@@ -6101,7 +6101,7 @@
         <v>8.378029931067296</v>
       </c>
       <c r="E333" t="n">
-        <v>0.3358963995827082</v>
+        <v>-0.3358963995827082</v>
       </c>
     </row>
     <row r="334">
@@ -6118,7 +6118,7 @@
         <v>7.297898710242766</v>
       </c>
       <c r="E334" t="n">
-        <v>0.4636162002363662</v>
+        <v>-0.4636162002363662</v>
       </c>
     </row>
     <row r="335">
@@ -6135,7 +6135,7 @@
         <v>7.769374844415283</v>
       </c>
       <c r="E335" t="n">
-        <v>-0.2585917152082189</v>
+        <v>0.2585917152082189</v>
       </c>
     </row>
     <row r="336">
@@ -6152,7 +6152,7 @@
         <v>6.9588774738582</v>
       </c>
       <c r="E336" t="n">
-        <v>0.2636948528851626</v>
+        <v>-0.2636948528851626</v>
       </c>
     </row>
     <row r="337">
@@ -6169,7 +6169,7 @@
         <v>8.0327210377098</v>
       </c>
       <c r="E337" t="n">
-        <v>0.1310894006077028</v>
+        <v>-0.1310894006077028</v>
       </c>
     </row>
     <row r="338">
@@ -6186,7 +6186,7 @@
         <v>7.948536904181504</v>
       </c>
       <c r="E338" t="n">
-        <v>-0.1623544155138017</v>
+        <v>0.1623544155138017</v>
       </c>
     </row>
     <row r="339">
@@ -6203,7 +6203,7 @@
         <v>6.934360299460297</v>
       </c>
       <c r="E339" t="n">
-        <v>0.4131835411928453</v>
+        <v>-0.4131835411928453</v>
       </c>
     </row>
     <row r="340">
@@ -6220,7 +6220,7 @@
         <v>7.066766513684604</v>
       </c>
       <c r="E340" t="n">
-        <v>-0.0135714585767488</v>
+        <v>0.0135714585767488</v>
       </c>
     </row>
     <row r="341">
@@ -6237,7 +6237,7 @@
         <v>8.002260049023603</v>
       </c>
       <c r="E341" t="n">
-        <v>-0.7556299272171021</v>
+        <v>0.7556299272171021</v>
       </c>
     </row>
     <row r="342">
@@ -6254,7 +6254,7 @@
         <v>7.943374704468254</v>
       </c>
       <c r="E342" t="n">
-        <v>-1.477582673585172</v>
+        <v>1.477582673585172</v>
       </c>
     </row>
     <row r="343">
@@ -6271,7 +6271,7 @@
         <v>7.178537268408901</v>
       </c>
       <c r="E343" t="n">
-        <v>-0.9616772195154422</v>
+        <v>0.9616772195154422</v>
       </c>
     </row>
     <row r="344">
@@ -6288,7 +6288,7 @@
         <v>7.996823626902396</v>
       </c>
       <c r="E344" t="n">
-        <v>-1.510448100589551</v>
+        <v>1.510448100589551</v>
       </c>
     </row>
     <row r="345">
@@ -6305,7 +6305,7 @@
         <v>7.819627635863841</v>
       </c>
       <c r="E345" t="n">
-        <v>-0.3834735431574909</v>
+        <v>0.3834735431574909</v>
       </c>
     </row>
     <row r="346">
@@ -6322,7 +6322,7 @@
         <v>7.987302196900257</v>
       </c>
       <c r="E346" t="n">
-        <v>-1.432184155116794</v>
+        <v>1.432184155116794</v>
       </c>
     </row>
     <row r="347">
@@ -6339,7 +6339,7 @@
         <v>7.228317732911652</v>
       </c>
       <c r="E347" t="n">
-        <v>-0.3463935487855547</v>
+        <v>0.3463935487855547</v>
       </c>
     </row>
     <row r="348">
@@ -6356,7 +6356,7 @@
         <v>7.592057278787493</v>
       </c>
       <c r="E348" t="n">
-        <v>-0.1890341409295857</v>
+        <v>0.1890341409295857</v>
       </c>
     </row>
     <row r="349">
@@ -6373,7 +6373,7 @@
         <v>6.507912599689724</v>
       </c>
       <c r="E349" t="n">
-        <v>-0.2150556079642225</v>
+        <v>0.2150556079642225</v>
       </c>
     </row>
     <row r="350">
@@ -6390,7 +6390,7 @@
         <v>5.906004076989301</v>
       </c>
       <c r="E350" t="n">
-        <v>-0.4743411281086747</v>
+        <v>0.4743411281086747</v>
       </c>
     </row>
     <row r="351">
@@ -6407,7 +6407,7 @@
         <v>5.838039608242701</v>
       </c>
       <c r="E351" t="n">
-        <v>-0.2006705391142489</v>
+        <v>0.2006705391142489</v>
       </c>
     </row>
     <row r="352">
@@ -6424,7 +6424,7 @@
         <v>6.309810822139716</v>
       </c>
       <c r="E352" t="n">
-        <v>-0.193948265192228</v>
+        <v>0.193948265192228</v>
       </c>
     </row>
     <row r="353">
@@ -6441,7 +6441,7 @@
         <v>6.781530776409341</v>
       </c>
       <c r="E353" t="n">
-        <v>0.414451229111398</v>
+        <v>-0.414451229111398</v>
       </c>
     </row>
     <row r="354">
@@ -6458,7 +6458,7 @@
         <v>8.302777622611533</v>
       </c>
       <c r="E354" t="n">
-        <v>0.4198441595911184</v>
+        <v>-0.4198441595911184</v>
       </c>
     </row>
     <row r="355">
@@ -6475,7 +6475,7 @@
         <v>8.842655335822787</v>
       </c>
       <c r="E355" t="n">
-        <v>0.4435742603253985</v>
+        <v>-0.4435742603253985</v>
       </c>
     </row>
     <row r="356">
@@ -6492,7 +6492,7 @@
         <v>8.502581789903822</v>
       </c>
       <c r="E356" t="n">
-        <v>0.1927431631807757</v>
+        <v>-0.1927431631807757</v>
       </c>
     </row>
     <row r="357">
@@ -6509,7 +6509,7 @@
         <v>8.324521286863497</v>
       </c>
       <c r="E357" t="n">
-        <v>0.1371204908906485</v>
+        <v>-0.1371204908906485</v>
       </c>
     </row>
     <row r="358">
@@ -6526,7 +6526,7 @@
         <v>7.2841762493336</v>
       </c>
       <c r="E358" t="n">
-        <v>0.2815062581144989</v>
+        <v>-0.2815062581144989</v>
       </c>
     </row>
     <row r="359">
@@ -6543,7 +6543,7 @@
         <v>7.903786258118211</v>
       </c>
       <c r="E359" t="n">
-        <v>-0.6590061537705605</v>
+        <v>0.6590061537705605</v>
       </c>
     </row>
     <row r="360">
@@ -6560,7 +6560,7 @@
         <v>8.095484697412695</v>
       </c>
       <c r="E360" t="n">
-        <v>-1.283679796746179</v>
+        <v>1.283679796746179</v>
       </c>
     </row>
     <row r="361">
@@ -6577,7 +6577,7 @@
         <v>8.244217027949112</v>
       </c>
       <c r="E361" t="n">
-        <v>-0.720987089903331</v>
+        <v>0.720987089903331</v>
       </c>
     </row>
     <row r="362">
@@ -6594,7 +6594,7 @@
         <v>7.488395979426486</v>
       </c>
       <c r="E362" t="n">
-        <v>-0.5351817592362025</v>
+        <v>0.5351817592362025</v>
       </c>
     </row>
     <row r="363">
@@ -6611,7 +6611,7 @@
         <v>8.168464301776371</v>
       </c>
       <c r="E363" t="n">
-        <v>-0.5614125078593881</v>
+        <v>0.5614125078593881</v>
       </c>
     </row>
     <row r="364">
@@ -6628,7 +6628,7 @@
         <v>9.44539945173997</v>
       </c>
       <c r="E364" t="n">
-        <v>-0.4772628331221327</v>
+        <v>0.4772628331221327</v>
       </c>
     </row>
     <row r="365">
@@ -6645,7 +6645,7 @@
         <v>8.868802988791158</v>
       </c>
       <c r="E365" t="n">
-        <v>-0.2304326524110785</v>
+        <v>0.2304326524110785</v>
       </c>
     </row>
     <row r="366">
@@ -6662,7 +6662,7 @@
         <v>9.107498246193847</v>
       </c>
       <c r="E366" t="n">
-        <v>-0.4849551151114184</v>
+        <v>0.4849551151114184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>